<commit_message>
updated version one more tree (fungi)
</commit_message>
<xml_diff>
--- a/trees_data.xlsx
+++ b/trees_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisfranciscohenaodiaz/Documents/UBC/Projects/MainFeaturesMacroEv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franciscohenaodiaz/Documents/UBC/Projects/MajorFeatsMacroEvol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DE2E49-92EC-BD49-B104-298EB29B84D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B33AD3-BA6B-6648-A3BC-AB648DA1F413}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15440" xr2:uid="{7E228B34-8B12-5E4D-8118-21C3676889E7}"/>
+    <workbookView xWindow="760" yWindow="860" windowWidth="25600" windowHeight="15440" xr2:uid="{7E228B34-8B12-5E4D-8118-21C3676889E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>study.id</t>
   </si>
@@ -273,6 +273,18 @@
       </rPr>
       <t>(2), 288.</t>
     </r>
+  </si>
+  <si>
+    <t>V2019</t>
+  </si>
+  <si>
+    <t>Vargaetal2019</t>
+  </si>
+  <si>
+    <t>Agaricomycetes</t>
+  </si>
+  <si>
+    <t>Fungi</t>
   </si>
 </sst>
 </file>
@@ -654,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9F6B5B-7B54-E74E-96D9-DD999532BC6A}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -774,95 +786,116 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1">
-        <v>9755</v>
+        <v>356305</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1">
-        <v>4007</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>1192</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1">
-        <v>356305</v>
+        <v>9755</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>1192</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>39</v>
+        <v>4007</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5284</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>